<commit_message>
created tc for diagnosis, gender, race, ethnicity
</commit_message>
<xml_diff>
--- a/InputFiles/TC01_Trials_Filter_Ethnicity-HispLatino.xlsx
+++ b/InputFiles/TC01_Trials_Filter_Ethnicity-HispLatino.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59E44F3C-2D32-4B82-B9E4-840E6750BF6A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D55015D-3C70-4AA1-AC25-DC5FABCB1B7C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="650" yWindow="1040" windowWidth="17860" windowHeight="7400" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="startup" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>WebExcel</t>
   </si>
@@ -49,6 +49,12 @@
   </si>
   <si>
     <t>MATCH (t:clinical_trial)&lt;--(a:arm)&lt;--(c:case)&lt;--(s:specimen)&lt;--(:assignment_report) WITH DISTINCT c AS c, t ,a, s WHERE c.ethnicity IN ['HISPANIC_OR_LATINO'] RETURN coalesce(c.case_id,'') AS `Case ID` , coalesce(t.clinical_trial_designation ,'')as `Trial Code` , coalesce(a.arm_id,'') As `Arm` , coalesce(a.arm_drug,'') As `Arm Treatment` , coalesce(c.disease,'') As Diagnosis , coalesce(c.gender,'') As Gender , coalesce(c.race,'') As Race , coalesce(c.ethnicity,'') As Ethnicity</t>
+  </si>
+  <si>
+    <t>StatQuery</t>
+  </si>
+  <si>
+    <t>MATCH (t:clinical_trial)&lt;--(a:arm)&lt;--(c:case)&lt;--(s:specimen)&lt;--(:assignment_report) WITH DISTINCT c AS c, t ,a, s WHERE c.ethnicity IN ['HISPANIC_OR_LATINO'] OPTIONAL MATCH (s)&lt;-[*]-(f:file) RETURN count(DISTINCT(f)) as number_of_files , count(DISTINCT(c.case_id)) as number_of_cases , count(DISTINCT(t.clinical_trial_designation)) as number_of_trial</t>
   </si>
 </sst>
 </file>
@@ -418,38 +424,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B2:B6"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="75.81640625" customWidth="1"/>
-    <col min="2" max="2" width="70.26953125" customWidth="1"/>
-    <col min="3" max="3" width="28.54296875" customWidth="1"/>
+    <col min="1" max="2" width="75.81640625" customWidth="1"/>
+    <col min="3" max="3" width="70.26953125" customWidth="1"/>
+    <col min="4" max="4" width="28.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="87" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" ht="87" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>